<commit_message>
feat(excel-finder) update project with searching files in defined directory and create sql-queries for repository
</commit_message>
<xml_diff>
--- a/data/1/МВС/!печать/З/МВС 2023.xlsx
+++ b/data/1/МВС/!печать/З/МВС 2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Студенческие\2023-24\МВС\!печать\З\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwlo\zachetker\data-sharer\data\1\МВС\!печать\З\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C06896-82C2-4DC7-9DC0-285D97FA3C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB166B57-5C2A-4999-ACFB-EAA00DF46A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Дневное" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="670">
   <si>
     <t>N_ZACHET</t>
   </si>
@@ -2476,23 +2476,23 @@
       <selection activeCell="I1" sqref="I1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>232001</v>
       </c>
@@ -2547,7 +2547,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>232002</v>
       </c>
@@ -2571,7 +2571,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>232003</v>
       </c>
@@ -2595,7 +2595,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>232004</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>232005</v>
       </c>
@@ -2643,7 +2643,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>232006</v>
       </c>
@@ -2667,7 +2667,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>232007</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>232008</v>
       </c>
@@ -2715,7 +2715,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>232009</v>
       </c>
@@ -2739,7 +2739,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>232010</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>232011</v>
       </c>
@@ -2787,7 +2787,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>232012</v>
       </c>
@@ -2811,7 +2811,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>232013</v>
       </c>
@@ -2835,7 +2835,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>232014</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>232015</v>
       </c>
@@ -2883,7 +2883,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>232016</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>232017</v>
       </c>
@@ -2931,7 +2931,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>232018</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>232019</v>
       </c>
@@ -2979,7 +2979,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>232020</v>
       </c>
@@ -3003,7 +3003,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>232021</v>
       </c>
@@ -3027,7 +3027,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>232022</v>
       </c>
@@ -3051,7 +3051,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>232023</v>
       </c>
@@ -3075,7 +3075,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>232024</v>
       </c>
@@ -3099,7 +3099,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>232025</v>
       </c>
@@ -3123,7 +3123,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>232026</v>
       </c>
@@ -3147,7 +3147,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>232027</v>
       </c>
@@ -3171,7 +3171,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>232028</v>
       </c>
@@ -3195,7 +3195,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>232029</v>
       </c>
@@ -3219,7 +3219,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>232030</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>232031</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>232032</v>
       </c>
@@ -3291,7 +3291,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>232033</v>
       </c>
@@ -3315,7 +3315,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>232034</v>
       </c>
@@ -3339,7 +3339,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>232035</v>
       </c>
@@ -3363,7 +3363,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="4"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>232036</v>
       </c>
@@ -3387,7 +3387,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>232037</v>
       </c>
@@ -3411,7 +3411,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>232038</v>
       </c>
@@ -3435,7 +3435,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>232039</v>
       </c>
@@ -3459,7 +3459,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>232040</v>
       </c>
@@ -3483,7 +3483,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>232041</v>
       </c>
@@ -3507,7 +3507,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>232042</v>
       </c>
@@ -3531,7 +3531,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>232043</v>
       </c>
@@ -3555,7 +3555,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>232044</v>
       </c>
@@ -3579,7 +3579,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>232045</v>
       </c>
@@ -3603,7 +3603,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>232046</v>
       </c>
@@ -3627,7 +3627,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="4"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>232047</v>
       </c>
@@ -3651,7 +3651,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="4"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>232048</v>
       </c>
@@ -3675,7 +3675,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="4"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>232071</v>
       </c>
@@ -3699,7 +3699,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="4"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>232072</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="4"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>232073</v>
       </c>
@@ -3747,7 +3747,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>232074</v>
       </c>
@@ -3771,7 +3771,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="4"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>232075</v>
       </c>
@@ -3795,7 +3795,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>232076</v>
       </c>
@@ -3819,7 +3819,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="4"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>232077</v>
       </c>
@@ -3843,7 +3843,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="4"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>232078</v>
       </c>
@@ -3867,7 +3867,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="4"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>232079</v>
       </c>
@@ -3891,7 +3891,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>232080</v>
       </c>
@@ -3915,7 +3915,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="4"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>232081</v>
       </c>
@@ -3939,7 +3939,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="4"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>232082</v>
       </c>
@@ -3963,7 +3963,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="4"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>232083</v>
       </c>
@@ -3987,7 +3987,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="4"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>232084</v>
       </c>
@@ -4011,7 +4011,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="4"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>232085</v>
       </c>
@@ -4035,7 +4035,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>232086</v>
       </c>
@@ -4059,7 +4059,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
         <v>232087</v>
       </c>
@@ -4083,7 +4083,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="4"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
         <v>232088</v>
       </c>
@@ -4107,7 +4107,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="4"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="7">
         <v>232089</v>
       </c>
@@ -4131,7 +4131,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="4"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="7">
         <v>232090</v>
       </c>
@@ -4155,7 +4155,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="4"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="7">
         <v>232091</v>
       </c>
@@ -4179,7 +4179,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="4"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="7">
         <v>232092</v>
       </c>
@@ -4203,7 +4203,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="4"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="7">
         <v>232093</v>
       </c>
@@ -4227,7 +4227,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="4"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="7">
         <v>232094</v>
       </c>
@@ -4251,7 +4251,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="4"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="7">
         <v>232095</v>
       </c>
@@ -4275,7 +4275,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="7">
         <v>232096</v>
       </c>
@@ -4299,7 +4299,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="4"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="7">
         <v>232097</v>
       </c>
@@ -4323,7 +4323,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="4"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="7">
         <v>232098</v>
       </c>
@@ -4347,7 +4347,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="4"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="7">
         <v>232099</v>
       </c>
@@ -4371,7 +4371,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="4"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="7">
         <v>232100</v>
       </c>
@@ -4395,7 +4395,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="4"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="7">
         <v>232101</v>
       </c>
@@ -4419,7 +4419,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="4"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="7">
         <v>232102</v>
       </c>
@@ -4443,7 +4443,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="4"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="7">
         <v>232103</v>
       </c>
@@ -4467,7 +4467,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="4"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="7">
         <v>232104</v>
       </c>
@@ -4491,7 +4491,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="4"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="7">
         <v>232105</v>
       </c>
@@ -4515,7 +4515,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="4"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="7">
         <v>232106</v>
       </c>
@@ -4539,7 +4539,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="4"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="7">
         <v>232107</v>
       </c>
@@ -4563,7 +4563,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="4"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="7">
         <v>232108</v>
       </c>
@@ -4587,7 +4587,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="4"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="7">
         <v>232109</v>
       </c>
@@ -4611,7 +4611,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="4"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="7">
         <v>232110</v>
       </c>
@@ -4635,7 +4635,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="4"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="7">
         <v>232111</v>
       </c>
@@ -4659,7 +4659,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="4"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
         <v>232112</v>
       </c>
@@ -4683,7 +4683,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="4"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="7">
         <v>232113</v>
       </c>
@@ -4707,7 +4707,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="4"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="7">
         <v>232114</v>
       </c>
@@ -4731,7 +4731,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="4"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="7">
         <v>232115</v>
       </c>
@@ -4755,7 +4755,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="4"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="7">
         <v>232116</v>
       </c>
@@ -4779,7 +4779,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="4"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="7">
         <v>232117</v>
       </c>
@@ -4803,7 +4803,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="4"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="7">
         <v>232118</v>
       </c>
@@ -4827,7 +4827,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="4"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="7">
         <v>232119</v>
       </c>
@@ -4851,7 +4851,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="4"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="7">
         <v>232120</v>
       </c>
@@ -4875,7 +4875,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="4"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="7">
         <v>232121</v>
       </c>
@@ -4899,7 +4899,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="4"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="7">
         <v>232122</v>
       </c>
@@ -4923,7 +4923,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="4"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="7">
         <v>232123</v>
       </c>
@@ -4947,7 +4947,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="4"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="7">
         <v>232124</v>
       </c>
@@ -4971,7 +4971,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="4"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="7">
         <v>232125</v>
       </c>
@@ -4995,7 +4995,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="4"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="7">
         <v>232126</v>
       </c>
@@ -5019,7 +5019,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="4"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="7">
         <v>232127</v>
       </c>
@@ -5043,7 +5043,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="4"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="7">
         <v>232128</v>
       </c>
@@ -5067,7 +5067,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="4"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="7">
         <v>232129</v>
       </c>
@@ -5091,7 +5091,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="4"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="7">
         <v>232130</v>
       </c>
@@ -5115,7 +5115,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="4"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="7">
         <v>232131</v>
       </c>
@@ -5139,7 +5139,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="4"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="7">
         <v>232132</v>
       </c>
@@ -5163,7 +5163,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="4"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="7">
         <v>232133</v>
       </c>
@@ -5187,7 +5187,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="4"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="7">
         <v>232134</v>
       </c>
@@ -5211,7 +5211,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="4"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="7">
         <v>232135</v>
       </c>
@@ -5235,7 +5235,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="4"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="7">
         <v>232136</v>
       </c>
@@ -5259,7 +5259,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="4"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="7">
         <v>232137</v>
       </c>
@@ -5283,7 +5283,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="4"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="7">
         <v>232138</v>
       </c>
@@ -5307,7 +5307,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="4"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="7">
         <v>232139</v>
       </c>
@@ -5331,7 +5331,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="4"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="7">
         <v>232140</v>
       </c>
@@ -5355,7 +5355,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="7">
         <v>232141</v>
       </c>
@@ -5379,7 +5379,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="4"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="7">
         <v>232142</v>
       </c>
@@ -5403,7 +5403,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="4"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="7">
         <v>232143</v>
       </c>
@@ -5427,7 +5427,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="4"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="7">
         <v>232144</v>
       </c>
@@ -5451,7 +5451,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="4"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="7">
         <v>232145</v>
       </c>
@@ -5475,7 +5475,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="4"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="7">
         <v>232146</v>
       </c>
@@ -5499,7 +5499,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="4"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="7">
         <v>232147</v>
       </c>
@@ -5523,7 +5523,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="7">
         <v>232148</v>
       </c>
@@ -5547,7 +5547,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="4"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="7">
         <v>232149</v>
       </c>
@@ -5571,7 +5571,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="4"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="7">
         <v>232150</v>
       </c>
@@ -5595,7 +5595,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="4"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="7">
         <v>232151</v>
       </c>
@@ -5619,7 +5619,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="4"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="7">
         <v>232152</v>
       </c>
@@ -5643,7 +5643,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="4"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="7">
         <v>232153</v>
       </c>
@@ -5667,7 +5667,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="4"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="7">
         <v>232154</v>
       </c>
@@ -5691,7 +5691,7 @@
       <c r="K133" s="3"/>
       <c r="L133" s="4"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="7">
         <v>232155</v>
       </c>
@@ -5715,7 +5715,7 @@
       <c r="K134" s="3"/>
       <c r="L134" s="4"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="7">
         <v>232156</v>
       </c>
@@ -5739,7 +5739,7 @@
       <c r="K135" s="3"/>
       <c r="L135" s="4"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="7">
         <v>232157</v>
       </c>
@@ -5763,7 +5763,7 @@
       <c r="K136" s="3"/>
       <c r="L136" s="4"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="7">
         <v>232158</v>
       </c>
@@ -5787,7 +5787,7 @@
       <c r="K137" s="3"/>
       <c r="L137" s="4"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="7">
         <v>232159</v>
       </c>
@@ -5811,7 +5811,7 @@
       <c r="K138" s="3"/>
       <c r="L138" s="4"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="7">
         <v>232160</v>
       </c>
@@ -5835,7 +5835,7 @@
       <c r="K139" s="3"/>
       <c r="L139" s="4"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="7">
         <v>232161</v>
       </c>
@@ -5859,7 +5859,7 @@
       <c r="K140" s="3"/>
       <c r="L140" s="4"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="7">
         <v>232162</v>
       </c>
@@ -5883,7 +5883,7 @@
       <c r="K141" s="3"/>
       <c r="L141" s="4"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="7">
         <v>232163</v>
       </c>
@@ -5907,7 +5907,7 @@
       <c r="K142" s="3"/>
       <c r="L142" s="4"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="7">
         <v>232164</v>
       </c>
@@ -5931,7 +5931,7 @@
       <c r="K143" s="3"/>
       <c r="L143" s="4"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="7">
         <v>232165</v>
       </c>
@@ -5955,7 +5955,7 @@
       <c r="K144" s="3"/>
       <c r="L144" s="4"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="7">
         <v>232166</v>
       </c>
@@ -5979,7 +5979,7 @@
       <c r="K145" s="3"/>
       <c r="L145" s="4"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="7">
         <v>232167</v>
       </c>
@@ -6003,7 +6003,7 @@
       <c r="K146" s="3"/>
       <c r="L146" s="4"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" s="7">
         <v>232168</v>
       </c>
@@ -6027,7 +6027,7 @@
       <c r="K147" s="3"/>
       <c r="L147" s="4"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="7">
         <v>232169</v>
       </c>
@@ -6051,7 +6051,7 @@
       <c r="K148" s="3"/>
       <c r="L148" s="4"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="7">
         <v>232170</v>
       </c>
@@ -6075,7 +6075,7 @@
       <c r="K149" s="3"/>
       <c r="L149" s="4"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" s="7">
         <v>232171</v>
       </c>
@@ -6099,7 +6099,7 @@
       <c r="K150" s="3"/>
       <c r="L150" s="4"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" s="7">
         <v>232172</v>
       </c>
@@ -6123,7 +6123,7 @@
       <c r="K151" s="3"/>
       <c r="L151" s="4"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" s="7">
         <v>232173</v>
       </c>
@@ -6147,7 +6147,7 @@
       <c r="K152" s="3"/>
       <c r="L152" s="4"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" s="7">
         <v>232174</v>
       </c>
@@ -6171,7 +6171,7 @@
       <c r="K153" s="3"/>
       <c r="L153" s="4"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" s="7">
         <v>232175</v>
       </c>
@@ -6195,7 +6195,7 @@
       <c r="K154" s="3"/>
       <c r="L154" s="4"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" s="7">
         <v>232176</v>
       </c>
@@ -6219,7 +6219,7 @@
       <c r="K155" s="3"/>
       <c r="L155" s="4"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" s="7">
         <v>232177</v>
       </c>
@@ -6243,7 +6243,7 @@
       <c r="K156" s="3"/>
       <c r="L156" s="4"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" s="7">
         <v>232178</v>
       </c>
@@ -6267,7 +6267,7 @@
       <c r="K157" s="3"/>
       <c r="L157" s="4"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" s="7">
         <v>232179</v>
       </c>
@@ -6291,7 +6291,7 @@
       <c r="K158" s="3"/>
       <c r="L158" s="4"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="7">
         <v>232180</v>
       </c>
@@ -6315,7 +6315,7 @@
       <c r="K159" s="3"/>
       <c r="L159" s="4"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" s="7">
         <v>232181</v>
       </c>
@@ -6339,7 +6339,7 @@
       <c r="K160" s="3"/>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="7">
         <v>232182</v>
       </c>
@@ -6363,7 +6363,7 @@
       <c r="K161" s="3"/>
       <c r="L161" s="4"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" s="7">
         <v>232183</v>
       </c>
@@ -6387,7 +6387,7 @@
       <c r="K162" s="3"/>
       <c r="L162" s="4"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" s="7">
         <v>232184</v>
       </c>
@@ -6411,7 +6411,7 @@
       <c r="K163" s="3"/>
       <c r="L163" s="4"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="7">
         <v>232185</v>
       </c>
@@ -6435,7 +6435,7 @@
       <c r="K164" s="3"/>
       <c r="L164" s="4"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="7">
         <v>232186</v>
       </c>
@@ -6459,7 +6459,7 @@
       <c r="K165" s="3"/>
       <c r="L165" s="4"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" s="7">
         <v>232187</v>
       </c>
@@ -6483,7 +6483,7 @@
       <c r="K166" s="3"/>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" s="7">
         <v>232188</v>
       </c>
@@ -6507,7 +6507,7 @@
       <c r="K167" s="3"/>
       <c r="L167" s="4"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" s="7">
         <v>232189</v>
       </c>
@@ -6531,7 +6531,7 @@
       <c r="K168" s="3"/>
       <c r="L168" s="4"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" s="7">
         <v>232190</v>
       </c>
@@ -6555,7 +6555,7 @@
       <c r="K169" s="3"/>
       <c r="L169" s="4"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" s="7">
         <v>232191</v>
       </c>
@@ -6579,7 +6579,7 @@
       <c r="K170" s="3"/>
       <c r="L170" s="4"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="7">
         <v>232192</v>
       </c>
@@ -6603,7 +6603,7 @@
       <c r="K171" s="3"/>
       <c r="L171" s="4"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" s="7">
         <v>232193</v>
       </c>
@@ -6627,7 +6627,7 @@
       <c r="K172" s="3"/>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" s="7">
         <v>232194</v>
       </c>
@@ -6651,7 +6651,7 @@
       <c r="K173" s="3"/>
       <c r="L173" s="4"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" s="7">
         <v>232195</v>
       </c>
@@ -6675,7 +6675,7 @@
       <c r="K174" s="3"/>
       <c r="L174" s="4"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="7">
         <v>232196</v>
       </c>
@@ -6699,7 +6699,7 @@
       <c r="K175" s="3"/>
       <c r="L175" s="4"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="7">
         <v>232197</v>
       </c>
@@ -6723,7 +6723,7 @@
       <c r="K176" s="3"/>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" s="7">
         <v>232198</v>
       </c>
@@ -6747,7 +6747,7 @@
       <c r="K177" s="3"/>
       <c r="L177" s="4"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" s="7">
         <v>232199</v>
       </c>
@@ -6771,7 +6771,7 @@
       <c r="K178" s="3"/>
       <c r="L178" s="4"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" s="7">
         <v>232200</v>
       </c>
@@ -6795,7 +6795,7 @@
       <c r="K179" s="3"/>
       <c r="L179" s="4"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" s="7">
         <v>232201</v>
       </c>
@@ -6819,7 +6819,7 @@
       <c r="K180" s="3"/>
       <c r="L180" s="4"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" s="7">
         <v>232203</v>
       </c>
@@ -6843,7 +6843,7 @@
       <c r="K181" s="3"/>
       <c r="L181" s="4"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" s="7">
         <v>232204</v>
       </c>
@@ -6865,7 +6865,7 @@
       <c r="K182" s="3"/>
       <c r="L182" s="4"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" s="7">
         <v>232205</v>
       </c>
@@ -6887,7 +6887,7 @@
       <c r="K183" s="3"/>
       <c r="L183" s="4"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" s="7">
         <v>232206</v>
       </c>
@@ -6909,7 +6909,7 @@
       <c r="K184" s="3"/>
       <c r="L184" s="4"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" s="7">
         <v>232207</v>
       </c>
@@ -6931,7 +6931,7 @@
       <c r="K185" s="3"/>
       <c r="L185" s="4"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" s="7">
         <v>232208</v>
       </c>
@@ -6953,7 +6953,7 @@
       <c r="K186" s="3"/>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" s="7">
         <v>232209</v>
       </c>
@@ -6975,7 +6975,7 @@
       <c r="K187" s="3"/>
       <c r="L187" s="4"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" s="7">
         <v>232210</v>
       </c>
@@ -6997,7 +6997,7 @@
       <c r="K188" s="3"/>
       <c r="L188" s="4"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" s="7">
         <v>232211</v>
       </c>
@@ -7019,7 +7019,7 @@
       <c r="K189" s="3"/>
       <c r="L189" s="4"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" s="7">
         <v>232212</v>
       </c>
@@ -7041,7 +7041,7 @@
       <c r="K190" s="3"/>
       <c r="L190" s="4"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" s="7">
         <v>232213</v>
       </c>
@@ -7063,7 +7063,7 @@
       <c r="K191" s="3"/>
       <c r="L191" s="4"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" s="7">
         <v>232214</v>
       </c>
@@ -7085,7 +7085,7 @@
       <c r="K192" s="3"/>
       <c r="L192" s="4"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" s="7">
         <v>232215</v>
       </c>
@@ -7107,7 +7107,7 @@
       <c r="K193" s="3"/>
       <c r="L193" s="4"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" s="7">
         <v>232216</v>
       </c>
@@ -7129,7 +7129,7 @@
       <c r="K194" s="3"/>
       <c r="L194" s="4"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" s="7">
         <v>232217</v>
       </c>
@@ -7151,7 +7151,7 @@
       <c r="K195" s="3"/>
       <c r="L195" s="4"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" s="7">
         <v>232218</v>
       </c>
@@ -7173,7 +7173,7 @@
       <c r="K196" s="3"/>
       <c r="L196" s="4"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197" s="7">
         <v>232219</v>
       </c>
@@ -7195,7 +7195,7 @@
       <c r="K197" s="3"/>
       <c r="L197" s="4"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198" s="7">
         <v>232220</v>
       </c>
@@ -7217,7 +7217,7 @@
       <c r="K198" s="3"/>
       <c r="L198" s="4"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A199" s="7">
         <v>232221</v>
       </c>
@@ -7239,7 +7239,7 @@
       <c r="K199" s="3"/>
       <c r="L199" s="4"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200" s="7">
         <v>232222</v>
       </c>
@@ -7261,7 +7261,7 @@
       <c r="K200" s="3"/>
       <c r="L200" s="4"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201" s="7">
         <v>232223</v>
       </c>
@@ -7283,7 +7283,7 @@
       <c r="K201" s="3"/>
       <c r="L201" s="4"/>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A202" s="7">
         <v>232224</v>
       </c>
@@ -7305,7 +7305,7 @@
       <c r="K202" s="3"/>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A203" s="7">
         <v>232225</v>
       </c>
@@ -7327,7 +7327,7 @@
       <c r="K203" s="3"/>
       <c r="L203" s="4"/>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A204" s="7">
         <v>232226</v>
       </c>
@@ -7349,7 +7349,7 @@
       <c r="K204" s="3"/>
       <c r="L204" s="4"/>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A205" s="7">
         <v>232227</v>
       </c>
@@ -7371,7 +7371,7 @@
       <c r="K205" s="3"/>
       <c r="L205" s="4"/>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A206" s="7">
         <v>232228</v>
       </c>
@@ -7393,7 +7393,7 @@
       <c r="K206" s="3"/>
       <c r="L206" s="4"/>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207" s="7">
         <v>232229</v>
       </c>
@@ -7415,7 +7415,7 @@
       <c r="K207" s="3"/>
       <c r="L207" s="4"/>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A208" s="7">
         <v>232230</v>
       </c>
@@ -7437,7 +7437,7 @@
       <c r="K208" s="3"/>
       <c r="L208" s="4"/>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" s="7">
         <v>232234</v>
       </c>
@@ -7461,7 +7461,7 @@
       <c r="K209" s="3"/>
       <c r="L209" s="4"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" s="7">
         <v>232235</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="K210" s="3"/>
       <c r="L210" s="4"/>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211" s="7">
         <v>232236</v>
       </c>
@@ -7509,7 +7509,7 @@
       <c r="K211" s="3"/>
       <c r="L211" s="4"/>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" s="7">
         <v>232237</v>
       </c>
@@ -7533,7 +7533,7 @@
       <c r="K212" s="3"/>
       <c r="L212" s="4"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213" s="7">
         <v>232238</v>
       </c>
@@ -7557,7 +7557,7 @@
       <c r="K213" s="3"/>
       <c r="L213" s="4"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" s="7">
         <v>232239</v>
       </c>
@@ -7581,7 +7581,7 @@
       <c r="K214" s="3"/>
       <c r="L214" s="4"/>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" s="7">
         <v>232240</v>
       </c>
@@ -7605,7 +7605,7 @@
       <c r="K215" s="3"/>
       <c r="L215" s="4"/>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" s="7">
         <v>232241</v>
       </c>
@@ -7629,7 +7629,7 @@
       <c r="K216" s="3"/>
       <c r="L216" s="4"/>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217" s="7">
         <v>232242</v>
       </c>
@@ -7653,7 +7653,7 @@
       <c r="K217" s="3"/>
       <c r="L217" s="4"/>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218" s="7">
         <v>232243</v>
       </c>
@@ -7677,7 +7677,7 @@
       <c r="K218" s="3"/>
       <c r="L218" s="4"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" s="7">
         <v>232244</v>
       </c>
@@ -7701,7 +7701,7 @@
       <c r="K219" s="3"/>
       <c r="L219" s="4"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" s="7">
         <v>232245</v>
       </c>
@@ -7725,7 +7725,7 @@
       <c r="K220" s="3"/>
       <c r="L220" s="4"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" s="7">
         <v>232246</v>
       </c>
@@ -7749,7 +7749,7 @@
       <c r="K221" s="3"/>
       <c r="L221" s="4"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" s="7">
         <v>232247</v>
       </c>
@@ -7773,7 +7773,7 @@
       <c r="K222" s="3"/>
       <c r="L222" s="4"/>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" s="7">
         <v>232248</v>
       </c>
@@ -7797,7 +7797,7 @@
       <c r="K223" s="3"/>
       <c r="L223" s="4"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" s="7">
         <v>232249</v>
       </c>
@@ -7821,7 +7821,7 @@
       <c r="K224" s="3"/>
       <c r="L224" s="4"/>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225" s="7">
         <v>232250</v>
       </c>
@@ -7845,7 +7845,7 @@
       <c r="K225" s="3"/>
       <c r="L225" s="4"/>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226" s="7">
         <v>232251</v>
       </c>
@@ -7869,7 +7869,7 @@
       <c r="K226" s="3"/>
       <c r="L226" s="4"/>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A227" s="7">
         <v>232252</v>
       </c>
@@ -7893,7 +7893,7 @@
       <c r="K227" s="3"/>
       <c r="L227" s="4"/>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A228" s="7">
         <v>232253</v>
       </c>
@@ -7917,7 +7917,7 @@
       <c r="K228" s="3"/>
       <c r="L228" s="4"/>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229" s="7">
         <v>232254</v>
       </c>
@@ -7941,7 +7941,7 @@
       <c r="K229" s="3"/>
       <c r="L229" s="4"/>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230" s="7">
         <v>232255</v>
       </c>
@@ -7965,7 +7965,7 @@
       <c r="K230" s="3"/>
       <c r="L230" s="4"/>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A231" s="7">
         <v>232256</v>
       </c>
@@ -7989,7 +7989,7 @@
       <c r="K231" s="3"/>
       <c r="L231" s="4"/>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232" s="7">
         <v>232257</v>
       </c>
@@ -8013,7 +8013,7 @@
       <c r="K232" s="3"/>
       <c r="L232" s="4"/>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A233" s="7">
         <v>232258</v>
       </c>
@@ -8037,7 +8037,7 @@
       <c r="K233" s="3"/>
       <c r="L233" s="4"/>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A234" s="7">
         <v>232259</v>
       </c>
@@ -8061,7 +8061,7 @@
       <c r="K234" s="3"/>
       <c r="L234" s="4"/>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235" s="7">
         <v>232260</v>
       </c>
@@ -8085,7 +8085,7 @@
       <c r="K235" s="3"/>
       <c r="L235" s="4"/>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A236" s="7">
         <v>232261</v>
       </c>
@@ -8109,7 +8109,7 @@
       <c r="K236" s="3"/>
       <c r="L236" s="4"/>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A237" s="7">
         <v>232262</v>
       </c>
@@ -8133,7 +8133,7 @@
       <c r="K237" s="3"/>
       <c r="L237" s="4"/>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A238" s="7">
         <v>232263</v>
       </c>
@@ -8157,7 +8157,7 @@
       <c r="K238" s="3"/>
       <c r="L238" s="4"/>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A239" s="7">
         <v>232264</v>
       </c>
@@ -8181,7 +8181,7 @@
       <c r="K239" s="3"/>
       <c r="L239" s="4"/>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A240" s="7">
         <v>232265</v>
       </c>
@@ -8205,7 +8205,7 @@
       <c r="K240" s="3"/>
       <c r="L240" s="4"/>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A241" s="7">
         <v>232266</v>
       </c>
@@ -8229,7 +8229,7 @@
       <c r="K241" s="3"/>
       <c r="L241" s="4"/>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" s="7">
         <v>232267</v>
       </c>
@@ -8253,7 +8253,7 @@
       <c r="K242" s="3"/>
       <c r="L242" s="4"/>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" s="7">
         <v>232268</v>
       </c>
@@ -8277,7 +8277,7 @@
       <c r="K243" s="3"/>
       <c r="L243" s="4"/>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" s="7">
         <v>232269</v>
       </c>
@@ -8301,7 +8301,7 @@
       <c r="K244" s="3"/>
       <c r="L244" s="4"/>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" s="7">
         <v>232270</v>
       </c>
@@ -8325,7 +8325,7 @@
       <c r="K245" s="3"/>
       <c r="L245" s="4"/>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" s="7">
         <v>232271</v>
       </c>
@@ -8349,7 +8349,7 @@
       <c r="K246" s="3"/>
       <c r="L246" s="4"/>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" s="7">
         <v>232272</v>
       </c>
@@ -8373,7 +8373,7 @@
       <c r="K247" s="3"/>
       <c r="L247" s="4"/>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" s="7">
         <v>232273</v>
       </c>
@@ -8397,7 +8397,7 @@
       <c r="K248" s="3"/>
       <c r="L248" s="4"/>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" s="7">
         <v>232274</v>
       </c>
@@ -8421,7 +8421,7 @@
       <c r="K249" s="3"/>
       <c r="L249" s="4"/>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" s="7">
         <v>232275</v>
       </c>
@@ -8445,7 +8445,7 @@
       <c r="K250" s="3"/>
       <c r="L250" s="4"/>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" s="7">
         <v>232276</v>
       </c>
@@ -8469,7 +8469,7 @@
       <c r="K251" s="3"/>
       <c r="L251" s="4"/>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" s="7">
         <v>232277</v>
       </c>
@@ -8491,7 +8491,7 @@
       <c r="K252" s="3"/>
       <c r="L252" s="4"/>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" s="7">
         <v>232278</v>
       </c>
@@ -8515,7 +8515,7 @@
       <c r="K253" s="3"/>
       <c r="L253" s="4"/>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" s="7">
         <v>232279</v>
       </c>
@@ -8539,7 +8539,7 @@
       <c r="K254" s="3"/>
       <c r="L254" s="4"/>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" s="7">
         <v>232280</v>
       </c>
@@ -8563,7 +8563,7 @@
       <c r="K255" s="3"/>
       <c r="L255" s="4"/>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" s="7">
         <v>232281</v>
       </c>
@@ -8587,7 +8587,7 @@
       <c r="K256" s="3"/>
       <c r="L256" s="4"/>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" s="7">
         <v>232282</v>
       </c>
@@ -8611,7 +8611,7 @@
       <c r="K257" s="3"/>
       <c r="L257" s="4"/>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258" s="7">
         <v>232283</v>
       </c>
@@ -8635,7 +8635,7 @@
       <c r="K258" s="3"/>
       <c r="L258" s="4"/>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259" s="7">
         <v>232284</v>
       </c>
@@ -8659,7 +8659,7 @@
       <c r="K259" s="3"/>
       <c r="L259" s="4"/>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" s="7">
         <v>232285</v>
       </c>
@@ -8683,7 +8683,7 @@
       <c r="K260" s="3"/>
       <c r="L260" s="4"/>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261" s="7">
         <v>232286</v>
       </c>
@@ -8707,7 +8707,7 @@
       <c r="K261" s="3"/>
       <c r="L261" s="4"/>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262" s="7">
         <v>232287</v>
       </c>
@@ -8731,7 +8731,7 @@
       <c r="K262" s="3"/>
       <c r="L262" s="4"/>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263" s="7">
         <v>232288</v>
       </c>
@@ -8755,7 +8755,7 @@
       <c r="K263" s="3"/>
       <c r="L263" s="4"/>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264" s="7">
         <v>232289</v>
       </c>
@@ -8779,7 +8779,7 @@
       <c r="K264" s="3"/>
       <c r="L264" s="4"/>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A265" s="7">
         <v>232290</v>
       </c>
@@ -8803,7 +8803,7 @@
       <c r="K265" s="3"/>
       <c r="L265" s="4"/>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266" s="7">
         <v>232291</v>
       </c>
@@ -8827,7 +8827,7 @@
       <c r="K266" s="3"/>
       <c r="L266" s="4"/>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A267" s="7">
         <v>232292</v>
       </c>
@@ -8851,7 +8851,7 @@
       <c r="K267" s="3"/>
       <c r="L267" s="4"/>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A268" s="7">
         <v>232293</v>
       </c>
@@ -8875,7 +8875,7 @@
       <c r="K268" s="3"/>
       <c r="L268" s="4"/>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A269" s="7">
         <v>232294</v>
       </c>
@@ -8899,7 +8899,7 @@
       <c r="K269" s="3"/>
       <c r="L269" s="4"/>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A270" s="7">
         <v>232295</v>
       </c>
@@ -8923,7 +8923,7 @@
       <c r="K270" s="3"/>
       <c r="L270" s="4"/>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A271" s="7">
         <v>232296</v>
       </c>
@@ -8947,7 +8947,7 @@
       <c r="K271" s="3"/>
       <c r="L271" s="4"/>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A272" s="7">
         <v>232297</v>
       </c>
@@ -8971,7 +8971,7 @@
       <c r="K272" s="3"/>
       <c r="L272" s="4"/>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A273" s="7">
         <v>232298</v>
       </c>
@@ -8995,7 +8995,7 @@
       <c r="K273" s="3"/>
       <c r="L273" s="4"/>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A274" s="7">
         <v>232299</v>
       </c>
@@ -9019,7 +9019,7 @@
       <c r="K274" s="3"/>
       <c r="L274" s="4"/>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A275" s="7">
         <v>232300</v>
       </c>
@@ -9043,7 +9043,7 @@
       <c r="K275" s="3"/>
       <c r="L275" s="4"/>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A276" s="7">
         <v>232301</v>
       </c>
@@ -9067,7 +9067,7 @@
       <c r="K276" s="3"/>
       <c r="L276" s="4"/>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A277" s="7">
         <v>232302</v>
       </c>
@@ -9091,7 +9091,7 @@
       <c r="K277" s="3"/>
       <c r="L277" s="4"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A278" s="7">
         <v>232303</v>
       </c>
@@ -9115,7 +9115,7 @@
       <c r="K278" s="3"/>
       <c r="L278" s="4"/>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A279" s="7">
         <v>232304</v>
       </c>
@@ -9139,7 +9139,7 @@
       <c r="K279" s="3"/>
       <c r="L279" s="4"/>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A280" s="7">
         <v>232305</v>
       </c>
@@ -9163,7 +9163,7 @@
       <c r="K280" s="3"/>
       <c r="L280" s="4"/>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A281" s="7">
         <v>232306</v>
       </c>
@@ -9187,7 +9187,7 @@
       <c r="K281" s="3"/>
       <c r="L281" s="4"/>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A282" s="7">
         <v>232307</v>
       </c>
@@ -9211,7 +9211,7 @@
       <c r="K282" s="3"/>
       <c r="L282" s="4"/>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A283" s="7">
         <v>232308</v>
       </c>
@@ -9235,7 +9235,7 @@
       <c r="K283" s="3"/>
       <c r="L283" s="4"/>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A284" s="7">
         <v>232309</v>
       </c>
@@ -9259,7 +9259,7 @@
       <c r="K284" s="3"/>
       <c r="L284" s="4"/>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A285" s="7">
         <v>232310</v>
       </c>
@@ -9300,25 +9300,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.88671875" style="1" customWidth="1"/>
     <col min="12" max="12" width="26" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="J1" s="2" t="s">
         <v>565</v>
       </c>
@@ -9329,7 +9332,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>232049</v>
       </c>
@@ -9361,7 +9364,7 @@
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>232050</v>
       </c>
@@ -9393,7 +9396,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>232051</v>
       </c>
@@ -9425,7 +9428,7 @@
       </c>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>232052</v>
       </c>
@@ -9457,7 +9460,7 @@
       </c>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>232053</v>
       </c>
@@ -9489,7 +9492,7 @@
       </c>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>232054</v>
       </c>
@@ -9521,7 +9524,7 @@
       </c>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>232055</v>
       </c>
@@ -9553,7 +9556,7 @@
       </c>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>232056</v>
       </c>
@@ -9585,7 +9588,7 @@
       </c>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>232057</v>
       </c>
@@ -9617,7 +9620,7 @@
       </c>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>232058</v>
       </c>
@@ -9649,7 +9652,7 @@
       </c>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>232059</v>
       </c>
@@ -9681,7 +9684,7 @@
       </c>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>232060</v>
       </c>
@@ -9713,7 +9716,7 @@
       </c>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>232061</v>
       </c>
@@ -9748,7 +9751,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>232062</v>
       </c>
@@ -9780,7 +9783,7 @@
       </c>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>232063</v>
       </c>
@@ -9812,7 +9815,7 @@
       </c>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>232064</v>
       </c>
@@ -9844,7 +9847,7 @@
       </c>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>232065</v>
       </c>
@@ -9876,7 +9879,7 @@
       </c>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>232066</v>
       </c>
@@ -9908,7 +9911,7 @@
       </c>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>232067</v>
       </c>
@@ -9940,7 +9943,7 @@
       </c>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>232068</v>
       </c>
@@ -9972,7 +9975,7 @@
       </c>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>232069</v>
       </c>
@@ -10004,7 +10007,7 @@
       </c>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>232070</v>
       </c>
@@ -10036,7 +10039,7 @@
       </c>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>232202</v>
       </c>
@@ -10068,7 +10071,7 @@
       </c>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>232231</v>
       </c>
@@ -10102,7 +10105,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>232232</v>
       </c>
@@ -10136,7 +10139,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>232233</v>
       </c>
@@ -10170,7 +10173,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>232311</v>
       </c>
@@ -10202,7 +10205,7 @@
       </c>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>232312</v>
       </c>
@@ -10234,7 +10237,7 @@
       </c>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>232313</v>
       </c>
@@ -10266,7 +10269,7 @@
       </c>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>232314</v>
       </c>
@@ -10298,7 +10301,7 @@
       </c>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>232315</v>
       </c>
@@ -10330,7 +10333,7 @@
       </c>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>232316</v>
       </c>
@@ -10362,7 +10365,7 @@
       </c>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>232317</v>
       </c>
@@ -10394,7 +10397,7 @@
       </c>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>232318</v>
       </c>
@@ -10426,7 +10429,7 @@
       </c>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>232319</v>
       </c>
@@ -10458,7 +10461,7 @@
       </c>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>232320</v>
       </c>
@@ -10490,7 +10493,7 @@
       </c>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>232321</v>
       </c>
@@ -10522,7 +10525,7 @@
       </c>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>232322</v>
       </c>
@@ -10554,7 +10557,7 @@
       </c>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>232323</v>
       </c>
@@ -10586,7 +10589,7 @@
       </c>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>232324</v>
       </c>
@@ -10618,7 +10621,7 @@
       </c>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>232325</v>
       </c>
@@ -10650,7 +10653,7 @@
       </c>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>232326</v>
       </c>
@@ -10682,7 +10685,7 @@
       </c>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>232327</v>
       </c>
@@ -10714,7 +10717,7 @@
       </c>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>232328</v>
       </c>
@@ -10746,7 +10749,7 @@
       </c>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>232329</v>
       </c>
@@ -10778,7 +10781,7 @@
       </c>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>232330</v>
       </c>
@@ -10810,7 +10813,7 @@
       </c>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>232331</v>
       </c>
@@ -10842,7 +10845,7 @@
       </c>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>232332</v>
       </c>
@@ -10874,7 +10877,7 @@
       </c>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>232333</v>
       </c>
@@ -10906,7 +10909,7 @@
       </c>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>232334</v>
       </c>
@@ -10938,7 +10941,7 @@
       </c>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>232335</v>
       </c>
@@ -10970,7 +10973,7 @@
       </c>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>232336</v>
       </c>
@@ -11002,7 +11005,7 @@
       </c>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>232337</v>
       </c>
@@ -11034,7 +11037,7 @@
       </c>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>232338</v>
       </c>
@@ -11066,7 +11069,7 @@
       </c>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>232339</v>
       </c>
@@ -11098,7 +11101,7 @@
       </c>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>232340</v>
       </c>
@@ -11130,7 +11133,7 @@
       </c>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>232341</v>
       </c>
@@ -11162,7 +11165,7 @@
       </c>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>232342</v>
       </c>
@@ -11194,7 +11197,7 @@
       </c>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>232343</v>
       </c>
@@ -11226,7 +11229,7 @@
       </c>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>232344</v>
       </c>
@@ -11258,7 +11261,7 @@
       </c>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>232345</v>
       </c>
@@ -11290,7 +11293,7 @@
       </c>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>232346</v>
       </c>
@@ -11322,7 +11325,7 @@
       </c>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>232347</v>
       </c>
@@ -11354,7 +11357,7 @@
       </c>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>232348</v>
       </c>
@@ -11386,7 +11389,7 @@
       </c>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
         <v>232349</v>
       </c>
@@ -11418,7 +11421,7 @@
       </c>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
         <v>232350</v>
       </c>
@@ -11450,7 +11453,7 @@
       </c>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="7">
         <v>232351</v>
       </c>
@@ -11482,7 +11485,7 @@
       </c>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="7">
         <v>232352</v>
       </c>
@@ -11514,7 +11517,7 @@
       </c>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="7">
         <v>232353</v>
       </c>
@@ -11546,7 +11549,7 @@
       </c>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="7">
         <v>232354</v>
       </c>
@@ -11578,7 +11581,7 @@
       </c>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="7">
         <v>232355</v>
       </c>
@@ -11610,7 +11613,7 @@
       </c>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="7">
         <v>232356</v>
       </c>
@@ -11642,7 +11645,7 @@
       </c>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="7">
         <v>232357</v>
       </c>
@@ -11674,7 +11677,7 @@
       </c>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="7">
         <v>232358</v>
       </c>
@@ -11706,7 +11709,7 @@
       </c>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="7">
         <v>232359</v>
       </c>
@@ -11738,7 +11741,7 @@
       </c>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="7">
         <v>232360</v>
       </c>
@@ -11770,7 +11773,7 @@
       </c>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="7">
         <v>232361</v>
       </c>
@@ -11802,7 +11805,7 @@
       </c>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="7">
         <v>232362</v>
       </c>
@@ -11834,7 +11837,7 @@
       </c>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="7">
         <v>232363</v>
       </c>
@@ -11866,7 +11869,7 @@
       </c>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="7">
         <v>232364</v>
       </c>
@@ -11898,7 +11901,7 @@
       </c>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="7">
         <v>232365</v>
       </c>
@@ -11930,7 +11933,7 @@
       </c>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="7">
         <v>232366</v>
       </c>
@@ -11962,7 +11965,7 @@
       </c>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="7">
         <v>232367</v>
       </c>
@@ -11994,7 +11997,7 @@
       </c>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="7">
         <v>232368</v>
       </c>
@@ -12026,7 +12029,7 @@
       </c>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="7">
         <v>232369</v>
       </c>
@@ -12058,7 +12061,7 @@
       </c>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="7">
         <v>232370</v>
       </c>
@@ -12090,7 +12093,7 @@
       </c>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="7">
         <v>232371</v>
       </c>

</xml_diff>